<commit_message>
Commit from Thursday 8/5 work session
</commit_message>
<xml_diff>
--- a/Pyomo_Excel.xlsx
+++ b/Pyomo_Excel.xlsx
@@ -8,14 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HValuck\Desktop\Pyomo Optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBA49ED-E1F7-49B7-9777-E41CC1759B65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338FEC8E-E3B1-4EA9-8F23-263D68AB7C8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28692" yWindow="-2460" windowWidth="24216" windowHeight="13116" activeTab="1" xr2:uid="{39CCFCBB-AF22-4DC3-A24B-93845F8E8F3C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="749" firstSheet="12" activeTab="22" xr2:uid="{39CCFCBB-AF22-4DC3-A24B-93845F8E8F3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Prod_Mix_Prob_Data" sheetId="2" r:id="rId1"/>
     <sheet name="Prod_Mix_Ch_DV" sheetId="3" r:id="rId2"/>
     <sheet name="Prod_Mix_Ch_Data" sheetId="4" r:id="rId3"/>
+    <sheet name="Proj_Sel_DV" sheetId="5" r:id="rId4"/>
+    <sheet name="Golf_Bags_Profit" sheetId="8" r:id="rId5"/>
+    <sheet name="Golf_Bags_Cons" sheetId="9" r:id="rId6"/>
+    <sheet name="BB_Gloves_Profit" sheetId="10" r:id="rId7"/>
+    <sheet name="BB_Gloves_Cons" sheetId="11" r:id="rId8"/>
+    <sheet name="BF_Cost" sheetId="12" r:id="rId9"/>
+    <sheet name="BF_Total" sheetId="14" r:id="rId10"/>
+    <sheet name="BF_Cons" sheetId="13" r:id="rId11"/>
+    <sheet name="IP_Yield" sheetId="15" r:id="rId12"/>
+    <sheet name="IP_Cons" sheetId="16" r:id="rId13"/>
+    <sheet name="IP_Amount" sheetId="20" r:id="rId14"/>
+    <sheet name="Proj_Sel_Data" sheetId="6" r:id="rId15"/>
+    <sheet name="Proj_Sel_Cons" sheetId="7" r:id="rId16"/>
+    <sheet name="PS_Rev" sheetId="21" r:id="rId17"/>
+    <sheet name="PS_Cost" sheetId="23" r:id="rId18"/>
+    <sheet name="PS_Cons" sheetId="22" r:id="rId19"/>
+    <sheet name="PS_MinMax" sheetId="24" r:id="rId20"/>
+    <sheet name="MD_Cost" sheetId="25" r:id="rId21"/>
+    <sheet name="MD_Capacity" sheetId="28" r:id="rId22"/>
+    <sheet name="MD_Demand" sheetId="26" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>Profit</t>
   </si>
@@ -69,19 +89,182 @@
   </si>
   <si>
     <t>Globs</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>FUNDS</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Deluxe</t>
+  </si>
+  <si>
+    <t>C_D</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>I_P</t>
+  </si>
+  <si>
+    <t>Fielder</t>
+  </si>
+  <si>
+    <t>Catcher</t>
+  </si>
+  <si>
+    <t>C_S</t>
+  </si>
+  <si>
+    <t>P_S</t>
+  </si>
+  <si>
+    <t>Professional</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Yards</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Yield</t>
+  </si>
+  <si>
+    <t>Risk</t>
+  </si>
+  <si>
+    <t>Proportion</t>
+  </si>
+  <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Money Market</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>M100</t>
+  </si>
+  <si>
+    <t>M200</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Operating</t>
+  </si>
+  <si>
+    <t>Chemical</t>
+  </si>
+  <si>
+    <t>Tacoma</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Tampa</t>
+  </si>
+  <si>
+    <t>Baltimore</t>
+  </si>
+  <si>
+    <t>Macon</t>
+  </si>
+  <si>
+    <t>Louisville</t>
+  </si>
+  <si>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>San_Diego</t>
+  </si>
+  <si>
+    <t>St_Louis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,9 +287,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,12 +694,773 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F32BCA1-FC0B-416F-ADB7-6B573E158878}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB415A0-F434-4D7F-82DA-176B0BD9C53B}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <v>0.3</v>
+      </c>
+      <c r="D2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>-0.06</v>
+      </c>
+      <c r="C3">
+        <v>-0.12</v>
+      </c>
+      <c r="D3">
+        <v>-0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99BFBCE8-F8DD-4DAC-9B15-99123C4AB4FD}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>0.2</v>
+      </c>
+      <c r="C2">
+        <v>0.1</v>
+      </c>
+      <c r="D2">
+        <v>0.06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8F6996-4BF8-4CCF-85F1-A68333A6E720}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <v>0.05</v>
+      </c>
+      <c r="D2">
+        <v>0.01</v>
+      </c>
+      <c r="E2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178F506B-5A68-42F6-9F53-0D6307C8EC0F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>1000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565A5F90-FAC9-4E4D-A26F-680B5DFA058A}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2">
+        <v>2016</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2017</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E1" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F1" s="2">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>400</v>
+      </c>
+      <c r="C2" s="2">
+        <v>230</v>
+      </c>
+      <c r="D2" s="2">
+        <v>330</v>
+      </c>
+      <c r="E2" s="2">
+        <v>400</v>
+      </c>
+      <c r="F2" s="2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>500</v>
+      </c>
+      <c r="C3" s="2">
+        <v>270</v>
+      </c>
+      <c r="D3" s="2">
+        <v>260</v>
+      </c>
+      <c r="E3" s="2">
+        <v>500</v>
+      </c>
+      <c r="F3" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>200</v>
+      </c>
+      <c r="C4" s="2">
+        <v>430</v>
+      </c>
+      <c r="D4" s="2">
+        <v>430</v>
+      </c>
+      <c r="E4" s="2">
+        <v>200</v>
+      </c>
+      <c r="F4" s="2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>300</v>
+      </c>
+      <c r="C5" s="2">
+        <v>220</v>
+      </c>
+      <c r="D5" s="2">
+        <v>270</v>
+      </c>
+      <c r="E5" s="2">
+        <v>300</v>
+      </c>
+      <c r="F5" s="2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>450</v>
+      </c>
+      <c r="C6" s="2">
+        <v>500</v>
+      </c>
+      <c r="D6" s="2">
+        <v>400</v>
+      </c>
+      <c r="E6" s="2">
+        <v>450</v>
+      </c>
+      <c r="F6" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>650</v>
+      </c>
+      <c r="C7" s="2">
+        <v>450</v>
+      </c>
+      <c r="D7" s="2">
+        <v>320</v>
+      </c>
+      <c r="E7" s="2">
+        <v>650</v>
+      </c>
+      <c r="F7" s="2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>350</v>
+      </c>
+      <c r="C8" s="2">
+        <v>530</v>
+      </c>
+      <c r="D8" s="2">
+        <v>330</v>
+      </c>
+      <c r="E8" s="2">
+        <v>350</v>
+      </c>
+      <c r="F8" s="2">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>300</v>
+      </c>
+      <c r="C9" s="2">
+        <v>700</v>
+      </c>
+      <c r="D9" s="2">
+        <v>260</v>
+      </c>
+      <c r="E9" s="2">
+        <v>300</v>
+      </c>
+      <c r="F9" s="2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>500</v>
+      </c>
+      <c r="C10" s="2">
+        <v>800</v>
+      </c>
+      <c r="D10" s="2">
+        <v>430</v>
+      </c>
+      <c r="E10" s="2">
+        <v>500</v>
+      </c>
+      <c r="F10" s="2">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>600</v>
+      </c>
+      <c r="C11" s="2">
+        <v>250</v>
+      </c>
+      <c r="D11" s="2">
+        <v>270</v>
+      </c>
+      <c r="E11" s="2">
+        <v>600</v>
+      </c>
+      <c r="F11" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>150</v>
+      </c>
+      <c r="C12" s="2">
+        <v>500</v>
+      </c>
+      <c r="D12" s="2">
+        <v>400</v>
+      </c>
+      <c r="E12" s="2">
+        <v>150</v>
+      </c>
+      <c r="F12" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>250</v>
+      </c>
+      <c r="C13" s="2">
+        <v>340</v>
+      </c>
+      <c r="D13" s="2">
+        <v>320</v>
+      </c>
+      <c r="E13" s="2">
+        <v>250</v>
+      </c>
+      <c r="F13" s="2">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>220</v>
+      </c>
+      <c r="C14" s="2">
+        <v>400</v>
+      </c>
+      <c r="D14" s="2">
+        <v>250</v>
+      </c>
+      <c r="E14" s="2">
+        <v>220</v>
+      </c>
+      <c r="F14" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>170</v>
+      </c>
+      <c r="C15" s="2">
+        <v>300</v>
+      </c>
+      <c r="D15" s="2">
+        <v>300</v>
+      </c>
+      <c r="E15" s="2">
+        <v>170</v>
+      </c>
+      <c r="F15" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>420</v>
+      </c>
+      <c r="C16" s="2">
+        <v>400</v>
+      </c>
+      <c r="D16" s="2">
+        <v>260</v>
+      </c>
+      <c r="E16" s="2">
+        <v>420</v>
+      </c>
+      <c r="F16" s="2">
+        <v>400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37751DF7-2D84-439A-B0DC-4F78AB0623B2}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3">
+        <v>2016</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2017</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2018</v>
+      </c>
+      <c r="E1" s="3">
+        <v>2019</v>
+      </c>
+      <c r="F1" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3">
+        <v>3500</v>
+      </c>
+      <c r="C2" s="3">
+        <v>4500</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4000</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3450</v>
+      </c>
+      <c r="F2" s="3">
+        <v>4500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A22FA45-BFEA-4696-9EBD-727B26D6E1C3}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>0.04</v>
+      </c>
+      <c r="C3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67119EF-2F0A-4194-B6BE-947E56CFF08F}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>75</v>
+      </c>
+      <c r="D2">
+        <f>0.04*B2</f>
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <f>0.025*C2</f>
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <f>B3*0.04*40</f>
+        <v>9.6</v>
+      </c>
+      <c r="E3">
+        <f>C3*0.025*50</f>
+        <v>7.5000000000000009</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{034A8865-592E-4620-A06E-537E255B3478}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D0C7C6-E020-4ABC-839A-E6097B2D366B}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -533,12 +1489,332 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACD38BF-E6C7-4042-95BE-D48D3D9E0F6C}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>375</v>
+      </c>
+      <c r="C2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>125</v>
+      </c>
+      <c r="C3">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8679E3F8-DBC5-4A22-BA2A-0C89A58505EA}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5"/>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2.75</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.85</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.85</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2.65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354C50ED-520C-4286-848A-B1F3AD4F2545}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="3">
+        <v>18000</v>
+      </c>
+      <c r="C2" s="3">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="3">
+        <v>15000</v>
+      </c>
+      <c r="C3" s="3">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="3">
+        <v>25000</v>
+      </c>
+      <c r="C4" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="3">
+        <v>20000</v>
+      </c>
+      <c r="C5" s="3">
+        <v>36.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5233B4-E18D-4279-8D6F-FE14EBFD52AA}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2">
+        <v>6800</v>
+      </c>
+      <c r="C2">
+        <v>11600</v>
+      </c>
+      <c r="D2">
+        <v>10800</v>
+      </c>
+      <c r="E2">
+        <v>10080</v>
+      </c>
+      <c r="F2">
+        <v>14400</v>
+      </c>
+      <c r="G2">
+        <v>12000</v>
+      </c>
+      <c r="H2">
+        <v>7200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BA3681-8BF0-44EB-BC4A-8FEF207FD110}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -585,4 +1861,400 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F94E986-741D-4DAD-856A-04D614AAD58E}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4DCC4C9-EE74-4E12-8BAD-02C14FFDE8AC}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27:I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D35A81-5960-4979-A59A-50C34DD9D09F}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>37800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>42480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>8100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954F38-F224-4D4B-B0A5-CA24990E9FCB}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB59AE7-D276-4767-9A0C-C328749D90F6}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>90</v>
+      </c>
+      <c r="D2">
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>12.5</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>6000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA03CE6D-B990-452D-BA85-E3D4C291780F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>7.5</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Friday 8/6 Work Session Commit - progress = nearly complete with Pet Food
</commit_message>
<xml_diff>
--- a/Pyomo_Excel.xlsx
+++ b/Pyomo_Excel.xlsx
@@ -8,25 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HValuck\Desktop\Pyomo Optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338FEC8E-E3B1-4EA9-8F23-263D68AB7C8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793F70D7-2E71-4BFE-BB39-F7CFCD8CFA3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="749" firstSheet="12" activeTab="22" xr2:uid="{39CCFCBB-AF22-4DC3-A24B-93845F8E8F3C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="749" firstSheet="22" activeTab="33" xr2:uid="{39CCFCBB-AF22-4DC3-A24B-93845F8E8F3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Prod_Mix_Prob_Data" sheetId="2" r:id="rId1"/>
     <sheet name="Prod_Mix_Ch_DV" sheetId="3" r:id="rId2"/>
     <sheet name="Prod_Mix_Ch_Data" sheetId="4" r:id="rId3"/>
-    <sheet name="Proj_Sel_DV" sheetId="5" r:id="rId4"/>
-    <sheet name="Golf_Bags_Profit" sheetId="8" r:id="rId5"/>
-    <sheet name="Golf_Bags_Cons" sheetId="9" r:id="rId6"/>
-    <sheet name="BB_Gloves_Profit" sheetId="10" r:id="rId7"/>
-    <sheet name="BB_Gloves_Cons" sheetId="11" r:id="rId8"/>
-    <sheet name="BF_Cost" sheetId="12" r:id="rId9"/>
-    <sheet name="BF_Total" sheetId="14" r:id="rId10"/>
-    <sheet name="BF_Cons" sheetId="13" r:id="rId11"/>
-    <sheet name="IP_Yield" sheetId="15" r:id="rId12"/>
-    <sheet name="IP_Cons" sheetId="16" r:id="rId13"/>
-    <sheet name="IP_Amount" sheetId="20" r:id="rId14"/>
+    <sheet name="Golf_Bags_Profit" sheetId="8" r:id="rId4"/>
+    <sheet name="Golf_Bags_Cons" sheetId="9" r:id="rId5"/>
+    <sheet name="BB_Gloves_Profit" sheetId="10" r:id="rId6"/>
+    <sheet name="BB_Gloves_Cons" sheetId="11" r:id="rId7"/>
+    <sheet name="BF_Cost" sheetId="12" r:id="rId8"/>
+    <sheet name="BF_Total" sheetId="14" r:id="rId9"/>
+    <sheet name="BF_Cons" sheetId="13" r:id="rId10"/>
+    <sheet name="IP_Yield" sheetId="15" r:id="rId11"/>
+    <sheet name="IP_Cons" sheetId="16" r:id="rId12"/>
+    <sheet name="IP_Amount" sheetId="20" r:id="rId13"/>
+    <sheet name="Proj_Sel_DV" sheetId="5" r:id="rId14"/>
     <sheet name="Proj_Sel_Data" sheetId="6" r:id="rId15"/>
     <sheet name="Proj_Sel_Cons" sheetId="7" r:id="rId16"/>
     <sheet name="PS_Rev" sheetId="21" r:id="rId17"/>
@@ -36,6 +36,17 @@
     <sheet name="MD_Cost" sheetId="25" r:id="rId21"/>
     <sheet name="MD_Capacity" sheetId="28" r:id="rId22"/>
     <sheet name="MD_Demand" sheetId="26" r:id="rId23"/>
+    <sheet name="CMR_Cost" sheetId="29" r:id="rId24"/>
+    <sheet name="CMR_Result" sheetId="30" r:id="rId25"/>
+    <sheet name="CMR_Cons" sheetId="32" r:id="rId26"/>
+    <sheet name="HS_Profit" sheetId="33" r:id="rId27"/>
+    <sheet name="HS_Cons" sheetId="34" r:id="rId28"/>
+    <sheet name="B_Profit" sheetId="36" r:id="rId29"/>
+    <sheet name="B_Cons" sheetId="37" r:id="rId30"/>
+    <sheet name="PF_Rev" sheetId="38" r:id="rId31"/>
+    <sheet name="PF_Cost" sheetId="40" r:id="rId32"/>
+    <sheet name="PF_Cons" sheetId="41" r:id="rId33"/>
+    <sheet name="PF_Prop" sheetId="39" r:id="rId34"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="92">
   <si>
     <t>Profit</t>
   </si>
@@ -239,13 +250,106 @@
   </si>
   <si>
     <t>St_Louis</t>
+  </si>
+  <si>
+    <t>Op_Cost</t>
+  </si>
+  <si>
+    <t>Limestone</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>Rough</t>
+  </si>
+  <si>
+    <t>Fine</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Coarse</t>
+  </si>
+  <si>
+    <t>Redi_Mix</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Face_Lift</t>
+  </si>
+  <si>
+    <t>Lipo</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Limit</t>
+  </si>
+  <si>
+    <t>Implant</t>
+  </si>
+  <si>
+    <t>Peanut_Butter</t>
+  </si>
+  <si>
+    <t>Apple_Butter</t>
+  </si>
+  <si>
+    <t>Sterilization</t>
+  </si>
+  <si>
+    <t>Packaging</t>
+  </si>
+  <si>
+    <t>Bird_Food</t>
+  </si>
+  <si>
+    <t>Dog_Food</t>
+  </si>
+  <si>
+    <t>Seeds</t>
+  </si>
+  <si>
+    <t>Stones</t>
+  </si>
+  <si>
+    <t>Cereal</t>
+  </si>
+  <si>
+    <t>Fishmeal</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Carbohydrates</t>
+  </si>
+  <si>
+    <t>Trace Minerals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abrasives </t>
+  </si>
+  <si>
+    <t>Blending</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Meat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -266,6 +370,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -275,9 +398,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -287,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -301,6 +433,23 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -695,34 +844,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F32BCA1-FC0B-416F-ADB7-6B573E158878}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB415A0-F434-4D7F-82DA-176B0BD9C53B}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -779,7 +900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99BFBCE8-F8DD-4DAC-9B15-99123C4AB4FD}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -822,7 +943,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8F6996-4BF8-4CCF-85F1-A68333A6E720}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -888,7 +1009,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178F506B-5A68-42F6-9F53-0D6307C8EC0F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -916,12 +1037,155 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F94E986-741D-4DAD-856A-04D614AAD58E}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565A5F90-FAC9-4E4D-A26F-680B5DFA058A}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1256,7 +1520,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1749,7 +2013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5233B4-E18D-4279-8D6F-FE14EBFD52AA}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1809,6 +2073,324 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F686A632-6F60-4975-924F-52B08DDA32A0}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DA4A89-F77F-4AB3-9C70-ED0037304D61}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="E2" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="E4" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="E5" s="6">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF5CA8D-B351-4FFD-9B08-6CD2C2334F79}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9201E4A2-39A6-4639-9E77-6D14527D8EF5}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>240</v>
+      </c>
+      <c r="C2">
+        <v>225</v>
+      </c>
+      <c r="D2">
+        <v>425</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6082C8C8-840B-4319-BEF2-B9CABB8CB827}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C67ABCD-7FBD-4864-8EF0-F42254E11BD4}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1100</v>
+      </c>
+      <c r="C2">
+        <v>1300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BA3681-8BF0-44EB-BC4A-8FEF207FD110}">
   <dimension ref="A1:D3"/>
@@ -1863,150 +2445,418 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D04D55B-FB0F-4711-BEFC-11189847AD66}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="8">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3047BB3D-56CF-411C-9772-B72A4EEEDE3C}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="9">
+        <v>750</v>
+      </c>
+      <c r="C2" s="9">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88341CB6-5BC7-4F29-B4A0-A102ED991FFE}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="6.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="12">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="12">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="12">
+        <v>900</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C343979B-4C17-4EC4-BB4F-3BE6C5E00B7C}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2">
+        <v>0.25</v>
+      </c>
+      <c r="C2">
+        <v>0.15</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
+      </c>
+      <c r="C3">
+        <v>0.3</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C1D732-FCBE-4A06-A9C6-5747DE2C3A5D}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="E2" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="F2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="12">
+        <v>0</v>
+      </c>
+      <c r="C3" s="12">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0.11</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F94E986-741D-4DAD-856A-04D614AAD58E}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2">
-        <v>4500</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4DCC4C9-EE74-4E12-8BAD-02C14FFDE8AC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2040,7 +2890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D35A81-5960-4979-A59A-50C34DD9D09F}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -2122,7 +2972,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954F38-F224-4D4B-B0A5-CA24990E9FCB}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2156,7 +3006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB59AE7-D276-4767-9A0C-C328749D90F6}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -2222,7 +3072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA03CE6D-B990-452D-BA85-E3D4C291780F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2257,4 +3107,32 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F32BCA1-FC0B-416F-ADB7-6B573E158878}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished through Pet Food
</commit_message>
<xml_diff>
--- a/Pyomo_Excel.xlsx
+++ b/Pyomo_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HValuck\Desktop\Pyomo Optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793F70D7-2E71-4BFE-BB39-F7CFCD8CFA3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9AEC70-0EF3-4D8E-80B3-5BD4B98B9311}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="749" firstSheet="22" activeTab="33" xr2:uid="{39CCFCBB-AF22-4DC3-A24B-93845F8E8F3C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="749" firstSheet="22" activeTab="23" xr2:uid="{39CCFCBB-AF22-4DC3-A24B-93845F8E8F3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Prod_Mix_Prob_Data" sheetId="2" r:id="rId1"/>
@@ -47,6 +47,9 @@
     <sheet name="PF_Cost" sheetId="40" r:id="rId32"/>
     <sheet name="PF_Cons" sheetId="41" r:id="rId33"/>
     <sheet name="PF_Prop" sheetId="39" r:id="rId34"/>
+    <sheet name="ES1_Cost" sheetId="42" r:id="rId35"/>
+    <sheet name="ES1_Cons" sheetId="43" r:id="rId36"/>
+    <sheet name="Sheet3" sheetId="44" r:id="rId37"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2077,7 +2080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F686A632-6F60-4975-924F-52B08DDA32A0}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -2509,7 +2512,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2627,7 +2630,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2685,13 +2688,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C1D732-FCBE-4A06-A9C6-5747DE2C3A5D}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="3" max="3" width="14.296875" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -2856,6 +2861,42 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCAFC49-7269-4D8F-A0E3-C2352024BCF2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A0806B-734F-4B4D-B8AE-F698B125798B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0400FE44-E48C-4E57-AE56-33161D68A49F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4DCC4C9-EE74-4E12-8BAD-02C14FFDE8AC}">
   <dimension ref="A1:C2"/>

</xml_diff>

<commit_message>
Complete Except for MPP and IM
</commit_message>
<xml_diff>
--- a/Pyomo_Excel.xlsx
+++ b/Pyomo_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HValuck\Desktop\Pyomo Optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9AEC70-0EF3-4D8E-80B3-5BD4B98B9311}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC1FBB9-D8DB-4DC8-8D69-B47C8A3DE8E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="749" firstSheet="22" activeTab="23" xr2:uid="{39CCFCBB-AF22-4DC3-A24B-93845F8E8F3C}"/>
+    <workbookView xWindow="2004" yWindow="2220" windowWidth="17280" windowHeight="8964" tabRatio="749" firstSheet="40" activeTab="48" xr2:uid="{39CCFCBB-AF22-4DC3-A24B-93845F8E8F3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Prod_Mix_Prob_Data" sheetId="2" r:id="rId1"/>
@@ -48,8 +48,20 @@
     <sheet name="PF_Cons" sheetId="41" r:id="rId33"/>
     <sheet name="PF_Prop" sheetId="39" r:id="rId34"/>
     <sheet name="ES1_Cost" sheetId="42" r:id="rId35"/>
-    <sheet name="ES1_Cons" sheetId="43" r:id="rId36"/>
-    <sheet name="Sheet3" sheetId="44" r:id="rId37"/>
+    <sheet name="ES1_Sched" sheetId="43" r:id="rId36"/>
+    <sheet name="LB_Cost" sheetId="45" r:id="rId37"/>
+    <sheet name="F_Profit" sheetId="47" r:id="rId38"/>
+    <sheet name="F_Cropcons" sheetId="48" r:id="rId39"/>
+    <sheet name="F_Farmcons" sheetId="49" r:id="rId40"/>
+    <sheet name="ID_Profit" sheetId="50" r:id="rId41"/>
+    <sheet name="ID_Cons" sheetId="51" r:id="rId42"/>
+    <sheet name="ES2_Cost" sheetId="52" r:id="rId43"/>
+    <sheet name="ES2_Cons" sheetId="53" r:id="rId44"/>
+    <sheet name="SR_Cost" sheetId="54" r:id="rId45"/>
+    <sheet name="SR_Cons" sheetId="55" r:id="rId46"/>
+    <sheet name="NF_Capacity" sheetId="56" r:id="rId47"/>
+    <sheet name="NF_Cost" sheetId="57" r:id="rId48"/>
+    <sheet name="NF_SupDem" sheetId="58" r:id="rId49"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -70,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="144">
   <si>
     <t>Profit</t>
   </si>
@@ -346,13 +358,169 @@
   </si>
   <si>
     <t>Meat</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>prob</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New York </t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>Midwest</t>
+  </si>
+  <si>
+    <t>Northeast</t>
+  </si>
+  <si>
+    <t>Northwest</t>
+  </si>
+  <si>
+    <t>Southeast</t>
+  </si>
+  <si>
+    <t>Southwest</t>
+  </si>
+  <si>
+    <t>CityFlag</t>
+  </si>
+  <si>
+    <t>Mid_Atlantic</t>
+  </si>
+  <si>
+    <t>Milo</t>
+  </si>
+  <si>
+    <t>Cotton</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>Acreage</t>
+  </si>
+  <si>
+    <t>Harvest</t>
+  </si>
+  <si>
+    <t>WaterCoeff</t>
+  </si>
+  <si>
+    <t>WaterCap</t>
+  </si>
+  <si>
+    <t>Weekender</t>
+  </si>
+  <si>
+    <t>Expedition</t>
+  </si>
+  <si>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Bilingual</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Katy</t>
+  </si>
+  <si>
+    <t>Wharton</t>
+  </si>
+  <si>
+    <t>Waha</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Carthage</t>
+  </si>
+  <si>
+    <t>Kiowa</t>
+  </si>
+  <si>
+    <t>Perryville</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Maumee</t>
+  </si>
+  <si>
+    <t>Joliet</t>
+  </si>
+  <si>
+    <t>Leidy</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Supply</t>
+  </si>
+  <si>
+    <t>Willingness to pay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -392,6 +560,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -422,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -454,6 +636,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2080,8 +2269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F686A632-6F60-4975-924F-52B08DDA32A0}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2863,36 +3052,752 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCAFC49-7269-4D8F-A0E3-C2352024BCF2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>655</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A0806B-734F-4B4D-B8AE-F698B125798B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9">
+        <v>1000</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+      <c r="D9">
+        <v>1000</v>
+      </c>
+      <c r="E9">
+        <v>1000</v>
+      </c>
+      <c r="F9">
+        <v>1000</v>
+      </c>
+      <c r="G9">
+        <v>1000</v>
+      </c>
+      <c r="H9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="13">
+        <v>14927</v>
+      </c>
+      <c r="C10" s="13">
+        <v>22123</v>
+      </c>
+      <c r="D10" s="13">
+        <v>18482</v>
+      </c>
+      <c r="E10" s="13">
+        <v>21088</v>
+      </c>
+      <c r="F10" s="13">
+        <v>19339</v>
+      </c>
+      <c r="G10" s="13">
+        <v>18174</v>
+      </c>
+      <c r="H10" s="13">
+        <v>13180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="13">
+        <v>1021</v>
+      </c>
+      <c r="C11" s="13">
+        <v>1508</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1126</v>
+      </c>
+      <c r="E11" s="13">
+        <v>1647</v>
+      </c>
+      <c r="F11" s="13">
+        <v>1812</v>
+      </c>
+      <c r="G11" s="13">
+        <v>952</v>
+      </c>
+      <c r="H11" s="13">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12">
+        <v>0.99</v>
+      </c>
+      <c r="C12">
+        <v>0.99</v>
+      </c>
+      <c r="D12">
+        <v>0.99</v>
+      </c>
+      <c r="E12">
+        <v>0.99</v>
+      </c>
+      <c r="F12">
+        <v>0.99</v>
+      </c>
+      <c r="G12">
+        <v>0.99</v>
+      </c>
+      <c r="H12">
+        <v>0.99</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0400FE44-E48C-4E57-AE56-33161D68A49F}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F07C108-FE58-413B-B30A-87433AEFDB14}">
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2">
+        <v>27000</v>
+      </c>
+      <c r="C2">
+        <v>13500</v>
+      </c>
+      <c r="D2">
+        <v>13500</v>
+      </c>
+      <c r="E2">
+        <v>13500</v>
+      </c>
+      <c r="F2">
+        <v>20250</v>
+      </c>
+      <c r="G2">
+        <v>20250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3">
+        <v>58500</v>
+      </c>
+      <c r="C3">
+        <v>39000</v>
+      </c>
+      <c r="D3">
+        <v>29250</v>
+      </c>
+      <c r="E3">
+        <v>39000</v>
+      </c>
+      <c r="F3">
+        <v>19500</v>
+      </c>
+      <c r="G3">
+        <v>19500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4">
+        <v>22500</v>
+      </c>
+      <c r="C4">
+        <v>15000</v>
+      </c>
+      <c r="D4">
+        <v>22500</v>
+      </c>
+      <c r="E4">
+        <v>15000</v>
+      </c>
+      <c r="F4">
+        <v>37500</v>
+      </c>
+      <c r="G4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5">
+        <v>81000</v>
+      </c>
+      <c r="C5">
+        <v>54000</v>
+      </c>
+      <c r="D5">
+        <v>27000</v>
+      </c>
+      <c r="E5">
+        <v>67500</v>
+      </c>
+      <c r="F5">
+        <v>27000</v>
+      </c>
+      <c r="G5">
+        <v>40500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6">
+        <v>21000</v>
+      </c>
+      <c r="C6">
+        <v>31500</v>
+      </c>
+      <c r="D6">
+        <v>52500</v>
+      </c>
+      <c r="E6">
+        <v>42000</v>
+      </c>
+      <c r="F6">
+        <v>63000</v>
+      </c>
+      <c r="G6">
+        <v>73500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7">
+        <v>84000</v>
+      </c>
+      <c r="C7">
+        <v>48000</v>
+      </c>
+      <c r="D7">
+        <v>36000</v>
+      </c>
+      <c r="E7">
+        <v>24000</v>
+      </c>
+      <c r="F7">
+        <v>48000</v>
+      </c>
+      <c r="G7">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8">
+        <v>18000</v>
+      </c>
+      <c r="C8">
+        <v>27000</v>
+      </c>
+      <c r="D8">
+        <v>54000</v>
+      </c>
+      <c r="E8">
+        <v>18000</v>
+      </c>
+      <c r="F8">
+        <v>63000</v>
+      </c>
+      <c r="G8">
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="3">
+        <v>25000</v>
+      </c>
+      <c r="C9" s="3">
+        <v>60000</v>
+      </c>
+      <c r="D9" s="3">
+        <v>35000</v>
+      </c>
+      <c r="E9" s="3">
+        <v>35000</v>
+      </c>
+      <c r="F9" s="3">
+        <v>30000</v>
+      </c>
+      <c r="G9" s="3">
+        <v>35000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9920547B-9B1F-4B1E-9DF0-FAA38BA86454}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>400</v>
+      </c>
+      <c r="C2">
+        <v>300</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>400</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>400</v>
+      </c>
+      <c r="C4">
+        <v>300</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4CF5F6-1731-4619-A1B9-640C8D467EE2}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3">
+        <v>700</v>
+      </c>
+      <c r="C3">
+        <v>800</v>
+      </c>
+      <c r="D3">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2924,6 +3829,2239 @@
       </c>
       <c r="C2">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4589953F-4068-4C66-92DE-30380B991C5B}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>400</v>
+      </c>
+      <c r="C2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>600</v>
+      </c>
+      <c r="C3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4">
+        <v>900</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33ADA0BD-C869-45CF-9E5B-33814865CAC8}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>3.8</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>1.5</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3331AAD-67B5-4624-8326-1EB348C6FFE6}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>12000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28CC5A1D-C8D8-4452-8EB2-405CA855DA53}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>7</v>
+      </c>
+      <c r="C1">
+        <v>8</v>
+      </c>
+      <c r="D1">
+        <v>9</v>
+      </c>
+      <c r="E1">
+        <v>10</v>
+      </c>
+      <c r="F1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25E7F01-2746-406F-A560-E3AF7C5F83BD}">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>7</v>
+      </c>
+      <c r="C1">
+        <v>8</v>
+      </c>
+      <c r="D1">
+        <v>9</v>
+      </c>
+      <c r="E1">
+        <v>10</v>
+      </c>
+      <c r="F1">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="14">
+        <v>5</v>
+      </c>
+      <c r="H2" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F11DE7A-801B-4AEE-B4D2-9C0ADCD338F6}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>52020</v>
+      </c>
+      <c r="C2">
+        <v>21420</v>
+      </c>
+      <c r="D2">
+        <v>74970</v>
+      </c>
+      <c r="E2">
+        <v>113220</v>
+      </c>
+      <c r="F2">
+        <v>142290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>36480</v>
+      </c>
+      <c r="C3">
+        <v>31920</v>
+      </c>
+      <c r="D3">
+        <v>126160.00000000003</v>
+      </c>
+      <c r="E3">
+        <v>138320</v>
+      </c>
+      <c r="F3">
+        <v>133760.00000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>21560</v>
+      </c>
+      <c r="C4">
+        <v>44660</v>
+      </c>
+      <c r="D4">
+        <v>56980.000000000015</v>
+      </c>
+      <c r="E4">
+        <v>144760.00000000003</v>
+      </c>
+      <c r="F4">
+        <v>132439.99999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>35880</v>
+      </c>
+      <c r="C5">
+        <v>49680</v>
+      </c>
+      <c r="D5">
+        <v>62100</v>
+      </c>
+      <c r="E5">
+        <v>113160</v>
+      </c>
+      <c r="F5">
+        <v>122820</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>19050</v>
+      </c>
+      <c r="C6">
+        <v>39370</v>
+      </c>
+      <c r="D6">
+        <v>26670</v>
+      </c>
+      <c r="E6">
+        <v>100330.00000000001</v>
+      </c>
+      <c r="F6">
+        <v>111760.00000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>54180.000000000015</v>
+      </c>
+      <c r="C7">
+        <v>63210</v>
+      </c>
+      <c r="D7">
+        <v>83850</v>
+      </c>
+      <c r="E7">
+        <v>99330.000000000015</v>
+      </c>
+      <c r="F7">
+        <v>78690</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>53280</v>
+      </c>
+      <c r="C8">
+        <v>68820</v>
+      </c>
+      <c r="D8">
+        <v>109890</v>
+      </c>
+      <c r="E8">
+        <v>68820</v>
+      </c>
+      <c r="F8">
+        <v>63270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>59400</v>
+      </c>
+      <c r="C9">
+        <v>66000</v>
+      </c>
+      <c r="D9">
+        <v>57200</v>
+      </c>
+      <c r="E9">
+        <v>83600</v>
+      </c>
+      <c r="F9">
+        <v>53900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>40300</v>
+      </c>
+      <c r="C10">
+        <v>53300</v>
+      </c>
+      <c r="D10">
+        <v>85800</v>
+      </c>
+      <c r="E10">
+        <v>97500</v>
+      </c>
+      <c r="F10">
+        <v>93600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>43200</v>
+      </c>
+      <c r="C11">
+        <v>87750</v>
+      </c>
+      <c r="D11">
+        <v>95850</v>
+      </c>
+      <c r="E11">
+        <v>81000</v>
+      </c>
+      <c r="F11">
+        <v>112050</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661E1280-7B05-4461-AF75-E62D134B39D7}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>153</v>
+      </c>
+      <c r="C2">
+        <v>153</v>
+      </c>
+      <c r="D2">
+        <v>153</v>
+      </c>
+      <c r="E2">
+        <v>153</v>
+      </c>
+      <c r="F2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>152</v>
+      </c>
+      <c r="C3">
+        <v>152</v>
+      </c>
+      <c r="D3">
+        <v>152</v>
+      </c>
+      <c r="E3">
+        <v>152</v>
+      </c>
+      <c r="F3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>154</v>
+      </c>
+      <c r="C4">
+        <v>154</v>
+      </c>
+      <c r="D4">
+        <v>154</v>
+      </c>
+      <c r="E4">
+        <v>154</v>
+      </c>
+      <c r="F4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>138</v>
+      </c>
+      <c r="C5">
+        <v>138</v>
+      </c>
+      <c r="D5">
+        <v>138</v>
+      </c>
+      <c r="E5">
+        <v>138</v>
+      </c>
+      <c r="F5">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>127</v>
+      </c>
+      <c r="C6">
+        <v>127</v>
+      </c>
+      <c r="D6">
+        <v>127</v>
+      </c>
+      <c r="E6">
+        <v>127</v>
+      </c>
+      <c r="F6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>129</v>
+      </c>
+      <c r="C7">
+        <v>129</v>
+      </c>
+      <c r="D7">
+        <v>129</v>
+      </c>
+      <c r="E7">
+        <v>129</v>
+      </c>
+      <c r="F7">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>111</v>
+      </c>
+      <c r="C8">
+        <v>111</v>
+      </c>
+      <c r="D8">
+        <v>111</v>
+      </c>
+      <c r="E8">
+        <v>111</v>
+      </c>
+      <c r="F8">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>110</v>
+      </c>
+      <c r="C9">
+        <v>110</v>
+      </c>
+      <c r="D9">
+        <v>110</v>
+      </c>
+      <c r="E9">
+        <v>110</v>
+      </c>
+      <c r="F9">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>130</v>
+      </c>
+      <c r="C10">
+        <v>130</v>
+      </c>
+      <c r="D10">
+        <v>130</v>
+      </c>
+      <c r="E10">
+        <v>130</v>
+      </c>
+      <c r="F10">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>135</v>
+      </c>
+      <c r="C11">
+        <v>135</v>
+      </c>
+      <c r="D11">
+        <v>135</v>
+      </c>
+      <c r="E11">
+        <v>135</v>
+      </c>
+      <c r="F11">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="2">
+        <v>350</v>
+      </c>
+      <c r="C12" s="2">
+        <v>250</v>
+      </c>
+      <c r="D12" s="2">
+        <v>500</v>
+      </c>
+      <c r="E12" s="2">
+        <v>400</v>
+      </c>
+      <c r="F12" s="2">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCF798B-FF07-4E33-93A0-E3637C06B70E}">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="15"/>
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+      <c r="I6">
+        <v>15</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>25</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>15</v>
+      </c>
+      <c r="L8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>15</v>
+      </c>
+      <c r="K9">
+        <v>20</v>
+      </c>
+      <c r="L9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>15</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>25</v>
+      </c>
+      <c r="L10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>15</v>
+      </c>
+      <c r="I11">
+        <v>20</v>
+      </c>
+      <c r="J11">
+        <v>25</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>15</v>
+      </c>
+      <c r="I12">
+        <v>30</v>
+      </c>
+      <c r="J12">
+        <v>25</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DA5E41-4360-47D9-A0A6-0100D7AC6356}">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="15"/>
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0.21</v>
+      </c>
+      <c r="D2">
+        <v>0.51</v>
+      </c>
+      <c r="E2">
+        <v>0.39</v>
+      </c>
+      <c r="F2">
+        <v>0.42</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3">
+        <v>0.21</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4">
+        <v>0.51</v>
+      </c>
+      <c r="C4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0.35</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5">
+        <v>0.39</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0.32</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6">
+        <v>0.42</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H6">
+        <v>0.3</v>
+      </c>
+      <c r="I6">
+        <v>0.35</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0.47</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.35</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.32</v>
+      </c>
+      <c r="F8">
+        <v>0.3</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0.48</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0.52</v>
+      </c>
+      <c r="L8">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.35</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0.48</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0.33</v>
+      </c>
+      <c r="K9">
+        <v>0.45</v>
+      </c>
+      <c r="L9">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0.33</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0.52</v>
+      </c>
+      <c r="L10">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.47</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.52</v>
+      </c>
+      <c r="I11">
+        <v>0.45</v>
+      </c>
+      <c r="J11">
+        <v>0.52</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0.22</v>
+      </c>
+      <c r="I12">
+        <v>0.47</v>
+      </c>
+      <c r="J12">
+        <v>0.53</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F870AA15-EB5C-43FF-A93C-F90BE1C1E142}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="16.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>35</v>
+      </c>
+      <c r="D11">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>60</v>
+      </c>
+      <c r="D12">
+        <v>4.63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished with all problems - need to reformat a few outputs for readability
</commit_message>
<xml_diff>
--- a/Pyomo_Excel.xlsx
+++ b/Pyomo_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HValuck\Desktop\Pyomo Optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C8E552-097F-4621-88CB-C4E026353D66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F0A010-6600-488C-B008-C4F1B845C18A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="749" firstSheet="40" activeTab="41" xr2:uid="{39CCFCBB-AF22-4DC3-A24B-93845F8E8F3C}"/>
+    <workbookView xWindow="1308" yWindow="2724" windowWidth="19836" windowHeight="9372" tabRatio="749" firstSheet="38" activeTab="42" xr2:uid="{39CCFCBB-AF22-4DC3-A24B-93845F8E8F3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Prod_Mix_Prob_Data" sheetId="2" r:id="rId1"/>
@@ -53,21 +53,22 @@
     <sheet name="F_Profit" sheetId="47" r:id="rId38"/>
     <sheet name="F_Cropcons" sheetId="48" r:id="rId39"/>
     <sheet name="F_Farmcons" sheetId="49" r:id="rId40"/>
-    <sheet name="IM_Day" sheetId="59" r:id="rId41"/>
-    <sheet name="IM_Cost" sheetId="60" r:id="rId42"/>
-    <sheet name="ID_Profit" sheetId="50" r:id="rId43"/>
-    <sheet name="ID_Cons" sheetId="51" r:id="rId44"/>
-    <sheet name="ES2_Cost" sheetId="52" r:id="rId45"/>
-    <sheet name="ES2_Cons" sheetId="53" r:id="rId46"/>
-    <sheet name="MPP_Profit" sheetId="62" r:id="rId47"/>
-    <sheet name="MPP_Cons" sheetId="61" r:id="rId48"/>
-    <sheet name="MPP_Props" sheetId="63" r:id="rId49"/>
-    <sheet name="MPP_Total" sheetId="64" r:id="rId50"/>
-    <sheet name="SR_Cost" sheetId="54" r:id="rId51"/>
-    <sheet name="SR_Cons" sheetId="55" r:id="rId52"/>
-    <sheet name="NF_Capacity" sheetId="56" r:id="rId53"/>
-    <sheet name="NF_Cost" sheetId="57" r:id="rId54"/>
-    <sheet name="NF_SupDem" sheetId="58" r:id="rId55"/>
+    <sheet name="IM_DV" sheetId="65" r:id="rId41"/>
+    <sheet name="IM_Demand" sheetId="59" r:id="rId42"/>
+    <sheet name="IM_Cost" sheetId="60" r:id="rId43"/>
+    <sheet name="ID_Profit" sheetId="50" r:id="rId44"/>
+    <sheet name="ID_Cons" sheetId="51" r:id="rId45"/>
+    <sheet name="ES2_Cost" sheetId="52" r:id="rId46"/>
+    <sheet name="ES2_Cons" sheetId="53" r:id="rId47"/>
+    <sheet name="MPP_Profit" sheetId="62" r:id="rId48"/>
+    <sheet name="MPP_Cons" sheetId="61" r:id="rId49"/>
+    <sheet name="MPP_Props" sheetId="63" r:id="rId50"/>
+    <sheet name="MPP_Total" sheetId="64" r:id="rId51"/>
+    <sheet name="SR_Cost" sheetId="54" r:id="rId52"/>
+    <sheet name="SR_Cons" sheetId="55" r:id="rId53"/>
+    <sheet name="NF_Capacity" sheetId="56" r:id="rId54"/>
+    <sheet name="NF_Cost" sheetId="57" r:id="rId55"/>
+    <sheet name="NF_SupDem" sheetId="58" r:id="rId56"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -88,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="186">
   <si>
     <t>Profit</t>
   </si>
@@ -522,87 +523,9 @@
     <t>Willingness to pay</t>
   </si>
   <si>
-    <t xml:space="preserve">Lights </t>
-  </si>
-  <si>
     <t>Heavies</t>
   </si>
   <si>
-    <t>Vehicle Type</t>
-  </si>
-  <si>
-    <t>Fixed</t>
-  </si>
-  <si>
-    <t>Variable</t>
-  </si>
-  <si>
-    <t>OL</t>
-  </si>
-  <si>
-    <t>OH</t>
-  </si>
-  <si>
-    <t>RL</t>
-  </si>
-  <si>
-    <t>RH</t>
-  </si>
-  <si>
-    <t>PC1</t>
-  </si>
-  <si>
-    <t>PCS</t>
-  </si>
-  <si>
-    <t>PC2</t>
-  </si>
-  <si>
-    <t>PH1</t>
-  </si>
-  <si>
-    <t>PHS</t>
-  </si>
-  <si>
-    <t>PH2</t>
-  </si>
-  <si>
-    <t>WC1</t>
-  </si>
-  <si>
-    <t>WCS</t>
-  </si>
-  <si>
-    <t>WC2</t>
-  </si>
-  <si>
-    <t>WH1</t>
-  </si>
-  <si>
-    <t>WHS</t>
-  </si>
-  <si>
-    <t>WH2</t>
-  </si>
-  <si>
-    <t>AC1</t>
-  </si>
-  <si>
-    <t>ACS</t>
-  </si>
-  <si>
-    <t>AC2</t>
-  </si>
-  <si>
-    <t>AH1</t>
-  </si>
-  <si>
-    <t>AHS</t>
-  </si>
-  <si>
-    <t>AH2</t>
-  </si>
-  <si>
     <t>Peanuts Purchased Month 1</t>
   </si>
   <si>
@@ -646,6 +569,84 @@
   </si>
   <si>
     <t>Chalet Month 2</t>
+  </si>
+  <si>
+    <t>Peanuts Chalet This Month</t>
+  </si>
+  <si>
+    <t>Peanuts Chalet Stored</t>
+  </si>
+  <si>
+    <t>Peanuts Chalet Next Month</t>
+  </si>
+  <si>
+    <t>Peanuts Hovel This Month</t>
+  </si>
+  <si>
+    <t>Peanuts Hovel Stored</t>
+  </si>
+  <si>
+    <t>Peanuts Hovel Next Month</t>
+  </si>
+  <si>
+    <t>Walnuts Chalet This Month</t>
+  </si>
+  <si>
+    <t>Walnuts Chalet Stored</t>
+  </si>
+  <si>
+    <t>Walnuts Chalet Next Month</t>
+  </si>
+  <si>
+    <t>Walnuts Hovel This Month</t>
+  </si>
+  <si>
+    <t>Walnuts Hovel Stored</t>
+  </si>
+  <si>
+    <t>Walnuts Hovel Next Month</t>
+  </si>
+  <si>
+    <t>Almonds Chalet This Month</t>
+  </si>
+  <si>
+    <t>Almonds Chalet Stored</t>
+  </si>
+  <si>
+    <t>Almonds Chalet Next Month</t>
+  </si>
+  <si>
+    <t>Almonds Hovel This Month</t>
+  </si>
+  <si>
+    <t>Almonds Hovel Stored</t>
+  </si>
+  <si>
+    <t>Almonds Hovel Next Month</t>
+  </si>
+  <si>
+    <t>Owned Heavies</t>
+  </si>
+  <si>
+    <t>Owned Lights</t>
+  </si>
+  <si>
+    <t>Used Lights</t>
+  </si>
+  <si>
+    <t>Rented Lights</t>
+  </si>
+  <si>
+    <t>Heavies as Lights</t>
+  </si>
+  <si>
+    <t>Used Heavies</t>
+  </si>
+  <si>
+    <t>Rented Heavies</t>
+  </si>
+  <si>
+    <t>Lights</t>
   </si>
 </sst>
 </file>
@@ -4051,20 +4052,71 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56421379-E472-40BF-9287-944A5CDE5BC5}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" customWidth="1"/>
+    <col min="4" max="4" width="16.69921875" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD790383-FDFA-431D-B7E2-901CE1D5ECA2}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="16"/>
       <c r="B1" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>144</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -4143,85 +4195,6 @@
       <c r="C8" s="14">
         <v>2</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87127CDA-3933-422B-80FE-E52CF1CFDCD9}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.09765625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="17">
-        <v>32</v>
-      </c>
-      <c r="C2" s="17">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="17">
-        <v>44</v>
-      </c>
-      <c r="C3" s="17">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" s="17">
-        <v>0</v>
-      </c>
-      <c r="C4" s="17">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5" s="17">
-        <v>0</v>
-      </c>
-      <c r="C5" s="17">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4229,11 +4202,98 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87127CDA-3933-422B-80FE-E52CF1CFDCD9}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.69921875" customWidth="1"/>
+    <col min="3" max="3" width="8.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="16"/>
+      <c r="B1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="16"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="17">
+        <v>44</v>
+      </c>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="17">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" s="17">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" s="17">
+        <v>40</v>
+      </c>
+      <c r="C6" s="18"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="17">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="17">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33ADA0BD-C869-45CF-9E5B-33814865CAC8}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4276,7 +4336,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3331AAD-67B5-4624-8326-1EB348C6FFE6}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -4349,7 +4409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28CC5A1D-C8D8-4452-8EB2-405CA855DA53}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -4421,7 +4481,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25E7F01-2746-406F-A560-E3AF7C5F83BD}">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -4797,17 +4857,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA12C2B-D6AC-473B-9A75-1CF585EA85C3}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.19921875" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -4817,7 +4880,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B2" s="1">
         <v>0.60000000000000009</v>
@@ -4825,7 +4888,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B3" s="1">
         <v>0.59000000000000008</v>
@@ -4833,7 +4896,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1">
         <v>0.62000000000000011</v>
@@ -4841,7 +4904,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B5" s="1">
         <v>0.2</v>
@@ -4849,7 +4912,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B6" s="1">
         <v>0.17</v>
@@ -4857,7 +4920,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B7" s="1">
         <v>0.2</v>
@@ -4865,7 +4928,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B8" s="1">
         <v>0.45000000000000007</v>
@@ -4873,7 +4936,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B9" s="1">
         <v>0.44000000000000006</v>
@@ -4881,7 +4944,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B10" s="1">
         <v>0.45000000000000007</v>
@@ -4889,7 +4952,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B11" s="1">
         <v>5.0000000000000044E-2</v>
@@ -4897,7 +4960,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B12" s="1">
         <v>2.0000000000000035E-2</v>
@@ -4905,7 +4968,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B13" s="1">
         <v>3.0000000000000027E-2</v>
@@ -4913,7 +4976,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B14" s="1">
         <v>0.30000000000000004</v>
@@ -4921,7 +4984,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B15" s="1">
         <v>0.29000000000000004</v>
@@ -4929,7 +4992,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B16" s="1">
         <v>0.29000000000000004</v>
@@ -4937,7 +5000,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B17" s="1">
         <v>-9.9999999999999978E-2</v>
@@ -4945,7 +5008,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B18" s="1">
         <v>-0.12999999999999998</v>
@@ -4953,7 +5016,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B19" s="1">
         <v>-0.13</v>
@@ -4964,12 +5027,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9515E66-1246-4906-91E0-603238F19102}">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4986,30 +5049,30 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
       <c r="C1" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="D1" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
       <c r="E1" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="F1" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="G1" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="H1" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -5035,7 +5098,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
@@ -5061,7 +5124,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B4" s="9">
         <v>0</v>
@@ -5087,7 +5150,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B5" s="9">
         <v>1</v>
@@ -5113,7 +5176,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B6" s="9">
         <v>1</v>
@@ -5139,7 +5202,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B7" s="9">
         <v>0</v>
@@ -5165,7 +5228,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B8" s="9">
         <v>0</v>
@@ -5191,7 +5254,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B9" s="9">
         <v>0</v>
@@ -5217,7 +5280,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B10" s="9">
         <v>0</v>
@@ -5243,7 +5306,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B11" s="9">
         <v>0</v>
@@ -5269,7 +5332,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B12" s="9">
         <v>0</v>
@@ -5295,7 +5358,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B13" s="9">
         <v>0</v>
@@ -5321,7 +5384,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B14" s="9">
         <v>0</v>
@@ -5347,7 +5410,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B15" s="9">
         <v>0</v>
@@ -5373,7 +5436,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B16" s="9">
         <v>0</v>
@@ -5399,7 +5462,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B17" s="9">
         <v>0</v>
@@ -5425,7 +5488,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B18" s="9">
         <v>0</v>
@@ -5451,7 +5514,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B19" s="9">
         <v>0</v>
@@ -5514,599 +5577,6 @@
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A0F264A-E793-4A7B-9B69-147383E04BD2}">
-  <dimension ref="A1:I21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.69921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H1" t="s">
-        <v>181</v>
-      </c>
-      <c r="I1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" s="9">
-        <v>-1</v>
-      </c>
-      <c r="C2" s="9">
-        <v>0</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0</v>
-      </c>
-      <c r="E2" s="9">
-        <v>0</v>
-      </c>
-      <c r="F2" s="9">
-        <v>0</v>
-      </c>
-      <c r="G2" s="9">
-        <v>0</v>
-      </c>
-      <c r="H2" s="9">
-        <v>0</v>
-      </c>
-      <c r="I2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="9">
-        <v>-1</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0</v>
-      </c>
-      <c r="E3" s="9">
-        <v>0</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0</v>
-      </c>
-      <c r="G3" s="9">
-        <v>0</v>
-      </c>
-      <c r="H3" s="9">
-        <v>0</v>
-      </c>
-      <c r="I3" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B4" s="9">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-      <c r="E4" s="9">
-        <v>0</v>
-      </c>
-      <c r="F4" s="9">
-        <v>-1</v>
-      </c>
-      <c r="G4" s="9">
-        <v>0</v>
-      </c>
-      <c r="H4" s="9">
-        <v>0</v>
-      </c>
-      <c r="I4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B5" s="9">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9">
-        <v>0</v>
-      </c>
-      <c r="F5" s="9">
-        <v>0</v>
-      </c>
-      <c r="G5" s="9">
-        <v>0</v>
-      </c>
-      <c r="H5" s="9">
-        <v>0</v>
-      </c>
-      <c r="I5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" s="9">
-        <v>0</v>
-      </c>
-      <c r="C6" s="9">
-        <v>-1</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0</v>
-      </c>
-      <c r="E6" s="9">
-        <v>0</v>
-      </c>
-      <c r="F6" s="9">
-        <v>0</v>
-      </c>
-      <c r="G6" s="9">
-        <v>0</v>
-      </c>
-      <c r="H6" s="9">
-        <v>0</v>
-      </c>
-      <c r="I6" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0</v>
-      </c>
-      <c r="E7" s="9">
-        <v>0</v>
-      </c>
-      <c r="F7" s="9">
-        <v>0</v>
-      </c>
-      <c r="G7" s="9">
-        <v>-1</v>
-      </c>
-      <c r="H7" s="9">
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>159</v>
-      </c>
-      <c r="B8" s="9">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0</v>
-      </c>
-      <c r="E8" s="9">
-        <v>0</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0</v>
-      </c>
-      <c r="G8" s="9">
-        <v>0</v>
-      </c>
-      <c r="H8" s="9">
-        <v>0</v>
-      </c>
-      <c r="I8" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>160</v>
-      </c>
-      <c r="B9" s="9">
-        <v>0</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="9">
-        <v>0</v>
-      </c>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>161</v>
-      </c>
-      <c r="B10" s="9">
-        <v>0</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0</v>
-      </c>
-      <c r="F10" s="9">
-        <v>0</v>
-      </c>
-      <c r="G10" s="9">
-        <v>0</v>
-      </c>
-      <c r="H10" s="9">
-        <v>0</v>
-      </c>
-      <c r="I10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B11" s="9">
-        <v>0</v>
-      </c>
-      <c r="C11" s="9">
-        <v>0</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0</v>
-      </c>
-      <c r="E11" s="9">
-        <v>0</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0</v>
-      </c>
-      <c r="G11" s="9">
-        <v>0</v>
-      </c>
-      <c r="H11" s="9">
-        <v>0</v>
-      </c>
-      <c r="I11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B12" s="9">
-        <v>0</v>
-      </c>
-      <c r="C12" s="9">
-        <v>0</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-      <c r="E12" s="9">
-        <v>0</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0</v>
-      </c>
-      <c r="G12" s="9">
-        <v>0</v>
-      </c>
-      <c r="H12" s="9">
-        <v>0</v>
-      </c>
-      <c r="I12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>164</v>
-      </c>
-      <c r="B13" s="9">
-        <v>0</v>
-      </c>
-      <c r="C13" s="9">
-        <v>0</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0</v>
-      </c>
-      <c r="E13" s="9">
-        <v>0</v>
-      </c>
-      <c r="F13" s="9">
-        <v>0</v>
-      </c>
-      <c r="G13" s="9">
-        <v>0</v>
-      </c>
-      <c r="H13" s="9">
-        <v>0</v>
-      </c>
-      <c r="I13" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>165</v>
-      </c>
-      <c r="B14" s="9">
-        <v>0</v>
-      </c>
-      <c r="C14" s="9">
-        <v>0</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1</v>
-      </c>
-      <c r="E14" s="9">
-        <v>0</v>
-      </c>
-      <c r="F14" s="9">
-        <v>0</v>
-      </c>
-      <c r="G14" s="9">
-        <v>0</v>
-      </c>
-      <c r="H14" s="9">
-        <v>0</v>
-      </c>
-      <c r="I14" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>166</v>
-      </c>
-      <c r="B15" s="9">
-        <v>0</v>
-      </c>
-      <c r="C15" s="9">
-        <v>0</v>
-      </c>
-      <c r="D15" s="9">
-        <v>1</v>
-      </c>
-      <c r="E15" s="9">
-        <v>0</v>
-      </c>
-      <c r="F15" s="9">
-        <v>0</v>
-      </c>
-      <c r="G15" s="9">
-        <v>0</v>
-      </c>
-      <c r="H15" s="9">
-        <v>0</v>
-      </c>
-      <c r="I15" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B16" s="9">
-        <v>0</v>
-      </c>
-      <c r="C16" s="9">
-        <v>0</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
-      <c r="E16" s="9">
-        <v>0</v>
-      </c>
-      <c r="F16" s="9">
-        <v>0</v>
-      </c>
-      <c r="G16" s="9">
-        <v>0</v>
-      </c>
-      <c r="H16" s="9">
-        <v>1</v>
-      </c>
-      <c r="I16" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B17" s="9">
-        <v>0</v>
-      </c>
-      <c r="C17" s="9">
-        <v>0</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0</v>
-      </c>
-      <c r="E17" s="9">
-        <v>1</v>
-      </c>
-      <c r="F17" s="9">
-        <v>0</v>
-      </c>
-      <c r="G17" s="9">
-        <v>0</v>
-      </c>
-      <c r="H17" s="9">
-        <v>0</v>
-      </c>
-      <c r="I17" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>169</v>
-      </c>
-      <c r="B18" s="9">
-        <v>0</v>
-      </c>
-      <c r="C18" s="9">
-        <v>0</v>
-      </c>
-      <c r="D18" s="9">
-        <v>0</v>
-      </c>
-      <c r="E18" s="9">
-        <v>1</v>
-      </c>
-      <c r="F18" s="9">
-        <v>0</v>
-      </c>
-      <c r="G18" s="9">
-        <v>0</v>
-      </c>
-      <c r="H18" s="9">
-        <v>0</v>
-      </c>
-      <c r="I18" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>170</v>
-      </c>
-      <c r="B19" s="9">
-        <v>0</v>
-      </c>
-      <c r="C19" s="9">
-        <v>0</v>
-      </c>
-      <c r="D19" s="9">
-        <v>0</v>
-      </c>
-      <c r="E19" s="9">
-        <v>0</v>
-      </c>
-      <c r="F19" s="9">
-        <v>0</v>
-      </c>
-      <c r="G19" s="9">
-        <v>0</v>
-      </c>
-      <c r="H19" s="9">
-        <v>0</v>
-      </c>
-      <c r="I19" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6196,11 +5666,604 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A0F264A-E793-4A7B-9B69-147383E04BD2}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0</v>
+      </c>
+      <c r="G2" s="9">
+        <v>0</v>
+      </c>
+      <c r="H2" s="9">
+        <v>0</v>
+      </c>
+      <c r="I2" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9">
+        <v>-1</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="9">
+        <v>0</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9">
+        <v>0</v>
+      </c>
+      <c r="I10" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9">
+        <v>0</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0</v>
+      </c>
+      <c r="I14" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0</v>
+      </c>
+      <c r="H16" s="9">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>175</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0</v>
+      </c>
+      <c r="I17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0</v>
+      </c>
+      <c r="I18" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0</v>
+      </c>
+      <c r="I19" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A399DE45-DCB8-42F4-AFE0-826559B1342B}">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6218,33 +6281,33 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="C1" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="D1" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="E1" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="F1" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="G1" t="s">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="H1" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="I1" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B2" s="9">
         <v>-1</v>
@@ -6273,7 +6336,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B3" s="9">
         <v>-1</v>
@@ -6302,7 +6365,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B4" s="9">
         <v>0</v>
@@ -6331,7 +6394,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B5" s="9">
         <v>0</v>
@@ -6360,7 +6423,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B6" s="9">
         <v>0</v>
@@ -6389,7 +6452,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B7" s="9">
         <v>0</v>
@@ -6418,7 +6481,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B8" s="9">
         <v>-1</v>
@@ -6447,7 +6510,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B9" s="9">
         <v>-1</v>
@@ -6476,7 +6539,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B10" s="9">
         <v>0</v>
@@ -6505,7 +6568,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B11" s="9">
         <v>0</v>
@@ -6534,7 +6597,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B12" s="9">
         <v>0</v>
@@ -6563,7 +6626,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B13" s="9">
         <v>0</v>
@@ -6592,7 +6655,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B14" s="9">
         <v>-1</v>
@@ -6621,7 +6684,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B15" s="9">
         <v>-1</v>
@@ -6650,7 +6713,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B16" s="9">
         <v>0</v>
@@ -6679,7 +6742,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B17" s="9">
         <v>0</v>
@@ -6708,7 +6771,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B18" s="9">
         <v>0</v>
@@ -6737,7 +6800,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B19" s="9">
         <v>0</v>
@@ -6812,7 +6875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F11DE7A-801B-4AEE-B4D2-9C0ADCD338F6}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -7044,7 +7107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661E1280-7B05-4461-AF75-E62D134B39D7}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -7296,7 +7359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCF798B-FF07-4E33-93A0-E3637C06B70E}">
   <dimension ref="A1:L12"/>
   <sheetViews>
@@ -7765,7 +7828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DA5E41-4360-47D9-A0A6-0100D7AC6356}">
   <dimension ref="A1:L12"/>
   <sheetViews>
@@ -8234,7 +8297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F870AA15-EB5C-43FF-A93C-F90BE1C1E142}">
   <dimension ref="A1:D12"/>
   <sheetViews>

</xml_diff>